<commit_message>
Add CSV and JSON join DuckDB example
</commit_message>
<xml_diff>
--- a/duckdb/duckdb_basics.xlsx
+++ b/duckdb/duckdb_basics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\xlslim-code-samples\duckdb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64DE897-9331-452F-B171-25A3DAE370EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9616A0-13CC-4FDE-8DD8-844F13FBD389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{10688695-ED20-49E9-B65B-C84E52F5D566}"/>
+    <workbookView xWindow="9797" yWindow="1509" windowWidth="20674" windowHeight="16277" xr2:uid="{10688695-ED20-49E9-B65B-C84E52F5D566}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Workbook location</t>
   </si>
@@ -122,6 +122,26 @@
   </si>
   <si>
     <t>https://duckdb.org/docs/data/parquet/overview</t>
+  </si>
+  <si>
+    <t>Querying both JSON and CSV</t>
+  </si>
+  <si>
+    <t>WITH CountrySales AS 
+(SELECT 
+    CASE WHEN Country='United States of America' THEN 'USA' ELSE Country END AS Country, 
+    Sum("Total Revenue") AS Sales 
+FROM 'D:\github\xlslim-code-samples\duckdb\..\data\10000SalesRecords.csv' 
+GROUP BY Country)
+SELECT 
+    cs.Country, 
+    SUM(cs.Sales) AS Sales, 
+    COUNT(*) AS "Nobel Laureates"
+FROM CountrySales cs
+INNER JOIN 'D:\github\xlslim-code-samples\duckdb\..\data\laureate.json' l
+ON cs.Country = l.bornCountry
+GROUP BY cs.Country
+ORDER BY "Nobel Laureates" DESC LIMIT 5</t>
   </si>
 </sst>
 </file>
@@ -211,7 +231,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -338,6 +358,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -348,7 +377,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="3" applyAlignment="1">
@@ -359,6 +388,11 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="3" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -369,9 +403,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -386,9 +417,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="40% - Accent4" xfId="4" builtinId="43"/>
@@ -778,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E9576C-E372-4400-8797-6F20E0DE1DCF}">
-  <dimension ref="A1:L81"/>
+  <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -792,7 +826,7 @@
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="102" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="13.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -800,17 +834,17 @@
         <f t="array" ref="B1">_xll.WorkbookLocation()</f>
         <v>D:\github\xlslim-code-samples\duckdb</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="13"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
@@ -820,15 +854,15 @@
         <f>B1&amp;"\..\data\10000SalesRecords.csv"</f>
         <v>D:\github\xlslim-code-samples\duckdb\..\data\10000SalesRecords.csv</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="13"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="15"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
@@ -838,15 +872,15 @@
         <f>B1&amp;"\..\data\laureate.json"</f>
         <v>D:\github\xlslim-code-samples\duckdb\..\data\laureate.json</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="13"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="15"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
@@ -856,18 +890,18 @@
         <f>B1&amp;"\..\data\titanic.parquet"</f>
         <v>D:\github\xlslim-code-samples\duckdb\..\data\titanic.parquet</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="18"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="8" t="s">
         <v>8</v>
       </c>
     </row>
@@ -891,14 +925,14 @@
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A9" s="18" t="str" cm="1">
+      <c r="A9" s="9" t="str" cm="1">
         <f t="array" ref="A9:C14">_xll.DuckDbQuery(A8)</f>
         <v>Region</v>
       </c>
-      <c r="B9" s="18" t="str">
+      <c r="B9" s="9" t="str">
         <v>Item Type</v>
       </c>
-      <c r="C9" s="18" t="str">
+      <c r="C9" s="9" t="str">
         <v>Total Revenue</v>
       </c>
     </row>
@@ -912,17 +946,17 @@
       <c r="C10" s="4">
         <v>2920025.64</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="10"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" t="str">
@@ -934,15 +968,15 @@
       <c r="C11" s="4">
         <v>51008.75</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="15"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" t="str">
@@ -954,15 +988,15 @@
       <c r="C12" s="4">
         <v>1003700.9</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="15"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" t="str">
@@ -974,15 +1008,15 @@
       <c r="C13" s="4">
         <v>5134318.41</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="18"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" t="str">
@@ -994,7 +1028,7 @@
       <c r="C14" s="4">
         <v>165647.95000000001</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1012,14 +1046,14 @@
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A18" s="18" t="str" cm="1">
+      <c r="A18" s="9" t="str" cm="1">
         <f t="array" ref="A18:C30">_xll.DuckDbQuery(A17)</f>
         <v>Item Type</v>
       </c>
-      <c r="B18" s="18" t="str">
+      <c r="B18" s="9" t="str">
         <v>Europe</v>
       </c>
-      <c r="C18" s="18" t="str">
+      <c r="C18" s="9" t="str">
         <v>Asia</v>
       </c>
     </row>
@@ -1033,17 +1067,17 @@
       <c r="C19" s="4">
         <v>169881436.88000003</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="10"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A20" t="str">
@@ -1055,15 +1089,15 @@
       <c r="C20" s="4">
         <v>26201083.349999994</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="15"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A21" t="str">
@@ -1075,15 +1109,15 @@
       <c r="C21" s="4">
         <v>124672713.00000007</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="15"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A22" t="str">
@@ -1095,15 +1129,15 @@
       <c r="C22" s="4">
         <v>57830320.320000023</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="15"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A23" t="str">
@@ -1115,15 +1149,15 @@
       <c r="C23" s="4">
         <v>260521796.39999998</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="15"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A24" t="str">
@@ -1135,15 +1169,15 @@
       <c r="C24" s="4">
         <v>4847196.24</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="15"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A25" t="str">
@@ -1155,15 +1189,15 @@
       <c r="C25" s="4">
         <v>394664223.51999986</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="15"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A26" t="str">
@@ -1175,7 +1209,7 @@
       <c r="C26" s="4">
         <v>240082410.95999998</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1227,7 +1261,7 @@
       <c r="A33" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="17" t="s">
+      <c r="D33" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1240,30 +1274,18 @@
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A36" s="18" t="str" cm="1">
+      <c r="A36" s="9" t="str" cm="1">
         <f t="array" ref="A36:C41">_xll.DuckDbQuery(A35)</f>
         <v>firstname</v>
       </c>
-      <c r="B36" s="18" t="str">
+      <c r="B36" s="9" t="str">
         <v>surname</v>
       </c>
-      <c r="C36" s="18" t="str">
+      <c r="C36" s="9" t="str">
         <v>bornCountry</v>
       </c>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A37" t="str">
@@ -1275,15 +1297,15 @@
       <c r="C37" t="str">
         <v>Prussia (now Germany)</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A38" t="str">
@@ -1295,13 +1317,13 @@
       <c r="C38" t="str">
         <v>the Netherlands</v>
       </c>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="12"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A39" t="str">
@@ -1313,13 +1335,13 @@
       <c r="C39" t="str">
         <v>the Netherlands</v>
       </c>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A40" t="str">
@@ -1331,13 +1353,13 @@
       <c r="C40" t="str">
         <v>France</v>
       </c>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="12"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A41" t="str">
@@ -1349,13 +1371,13 @@
       <c r="C41" t="str">
         <v>France</v>
       </c>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
     </row>
     <row r="44" spans="1:10" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A44" s="5" t="str">
@@ -1367,11 +1389,11 @@
       <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A45" s="18" t="str" cm="1">
+      <c r="A45" s="9" t="str" cm="1">
         <f t="array" ref="A45:B50">_xll.DuckDbQuery(A44)</f>
         <v>Country</v>
       </c>
-      <c r="B45" s="18" t="str">
+      <c r="B45" s="9" t="str">
         <v>Number</v>
       </c>
     </row>
@@ -1382,15 +1404,15 @@
       <c r="B46">
         <v>294</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
-      <c r="J46" s="12"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A47" t="str">
@@ -1399,13 +1421,13 @@
       <c r="B47">
         <v>91</v>
       </c>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
-      <c r="J47" s="12"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A48" t="str">
@@ -1414,13 +1436,13 @@
       <c r="B48">
         <v>67</v>
       </c>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
-      <c r="J48" s="12"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A49" t="str">
@@ -1449,17 +1471,17 @@
       <c r="E52" s="5"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A53" s="18" t="str" cm="1">
+      <c r="A53" s="9" t="str" cm="1">
         <f t="array" ref="A53:D58">_xll.DuckDbQuery(A52)</f>
         <v>firstname</v>
       </c>
-      <c r="B53" s="18" t="str">
+      <c r="B53" s="9" t="str">
         <v>surname</v>
       </c>
-      <c r="C53" s="18" t="str">
+      <c r="C53" s="9" t="str">
         <v>Category</v>
       </c>
-      <c r="D53" s="18" t="str">
+      <c r="D53" s="9" t="str">
         <v>Motivation</v>
       </c>
     </row>
@@ -1534,66 +1556,66 @@
       </c>
     </row>
     <row r="59" spans="1:10" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D59" s="12" t="s">
+      <c r="D59" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
-      <c r="H59" s="12"/>
-      <c r="I59" s="12"/>
-      <c r="J59" s="12"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
+      <c r="J59" s="10"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="12"/>
-      <c r="I60" s="12"/>
-      <c r="J60" s="12"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+      <c r="J60" s="10"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="12"/>
-      <c r="I61" s="12"/>
-      <c r="J61" s="12"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="10"/>
+      <c r="J61" s="10"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="12"/>
-      <c r="I62" s="12"/>
-      <c r="J62" s="12"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="10"/>
+      <c r="J62" s="10"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="12"/>
-      <c r="I63" s="12"/>
-      <c r="J63" s="12"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
+      <c r="J63" s="10"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="D64" s="12"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
-      <c r="H64" s="12"/>
-      <c r="I64" s="12"/>
-      <c r="J64" s="12"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
+      <c r="I64" s="10"/>
+      <c r="J64" s="10"/>
     </row>
     <row r="67" spans="1:10" ht="20.149999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A67" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D67" s="17" t="s">
+      <c r="D67" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1608,14 +1630,14 @@
       <c r="D69" s="5"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A70" s="18" t="str" cm="1">
+      <c r="A70" s="9" t="str" cm="1">
         <f t="array" ref="A70:C75">_xll.DuckDbQuery(A69)</f>
         <v>Survived</v>
       </c>
-      <c r="B70" s="18" t="str">
+      <c r="B70" s="9" t="str">
         <v>Pclass</v>
       </c>
-      <c r="C70" s="18" t="str">
+      <c r="C70" s="9" t="str">
         <v>Sex</v>
       </c>
     </row>
@@ -1629,15 +1651,15 @@
       <c r="C71" t="str">
         <v>male</v>
       </c>
-      <c r="D71" s="12" t="s">
+      <c r="D71" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
-      <c r="H71" s="12"/>
-      <c r="I71" s="12"/>
-      <c r="J71" s="12"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
+      <c r="I71" s="10"/>
+      <c r="J71" s="10"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A72">
@@ -1649,13 +1671,13 @@
       <c r="C72" t="str">
         <v>female</v>
       </c>
-      <c r="D72" s="12"/>
-      <c r="E72" s="12"/>
-      <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
-      <c r="H72" s="12"/>
-      <c r="I72" s="12"/>
-      <c r="J72" s="12"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
+      <c r="I72" s="10"/>
+      <c r="J72" s="10"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A73">
@@ -1667,13 +1689,13 @@
       <c r="C73" t="str">
         <v>female</v>
       </c>
-      <c r="D73" s="12"/>
-      <c r="E73" s="12"/>
-      <c r="F73" s="12"/>
-      <c r="G73" s="12"/>
-      <c r="H73" s="12"/>
-      <c r="I73" s="12"/>
-      <c r="J73" s="12"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
+      <c r="I73" s="10"/>
+      <c r="J73" s="10"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A74">
@@ -1685,13 +1707,13 @@
       <c r="C74" t="str">
         <v>female</v>
       </c>
-      <c r="D74" s="12"/>
-      <c r="E74" s="12"/>
-      <c r="F74" s="12"/>
-      <c r="G74" s="12"/>
-      <c r="H74" s="12"/>
-      <c r="I74" s="12"/>
-      <c r="J74" s="12"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="10"/>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10"/>
+      <c r="I74" s="10"/>
+      <c r="J74" s="10"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A75">
@@ -1703,13 +1725,13 @@
       <c r="C75" t="str">
         <v>male</v>
       </c>
-      <c r="D75" s="12"/>
-      <c r="E75" s="12"/>
-      <c r="F75" s="12"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="12"/>
-      <c r="I75" s="12"/>
-      <c r="J75" s="12"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="10"/>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
+      <c r="I75" s="10"/>
+      <c r="J75" s="10"/>
     </row>
     <row r="77" spans="1:10" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A77" s="5" t="str">
@@ -1718,33 +1740,33 @@
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
-      <c r="F77" s="12" t="s">
+      <c r="F77" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G77" s="12"/>
-      <c r="H77" s="12"/>
-      <c r="I77" s="12"/>
-      <c r="J77" s="12"/>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
+      <c r="I77" s="10"/>
+      <c r="J77" s="10"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A78" s="18" t="str" cm="1">
+      <c r="A78" s="9" t="str" cm="1">
         <f t="array" ref="A78:D80">_xll.DuckDbQuery(A77)</f>
         <v>Sex</v>
       </c>
-      <c r="B78" s="18" t="str">
+      <c r="B78" s="9" t="str">
         <v>1</v>
       </c>
-      <c r="C78" s="18" t="str">
+      <c r="C78" s="9" t="str">
         <v>2</v>
       </c>
-      <c r="D78" s="18" t="str">
+      <c r="D78" s="9" t="str">
         <v>3</v>
       </c>
-      <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
-      <c r="H78" s="12"/>
-      <c r="I78" s="12"/>
-      <c r="J78" s="12"/>
+      <c r="F78" s="10"/>
+      <c r="G78" s="10"/>
+      <c r="H78" s="10"/>
+      <c r="I78" s="10"/>
+      <c r="J78" s="10"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A79" t="str">
@@ -1759,11 +1781,11 @@
       <c r="D79">
         <v>47</v>
       </c>
-      <c r="F79" s="12"/>
-      <c r="G79" s="12"/>
-      <c r="H79" s="12"/>
-      <c r="I79" s="12"/>
-      <c r="J79" s="12"/>
+      <c r="F79" s="10"/>
+      <c r="G79" s="10"/>
+      <c r="H79" s="10"/>
+      <c r="I79" s="10"/>
+      <c r="J79" s="10"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A80" t="str">
@@ -1778,29 +1800,267 @@
       <c r="D80">
         <v>72</v>
       </c>
-      <c r="F80" s="12"/>
-      <c r="G80" s="12"/>
-      <c r="H80" s="12"/>
-      <c r="I80" s="12"/>
-      <c r="J80" s="12"/>
-    </row>
-    <row r="81" spans="6:10" x14ac:dyDescent="0.4">
-      <c r="F81" s="12"/>
-      <c r="G81" s="12"/>
-      <c r="H81" s="12"/>
-      <c r="I81" s="12"/>
-      <c r="J81" s="12"/>
+      <c r="F80" s="10"/>
+      <c r="G80" s="10"/>
+      <c r="H80" s="10"/>
+      <c r="I80" s="10"/>
+      <c r="J80" s="10"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="F81" s="10"/>
+      <c r="G81" s="10"/>
+      <c r="H81" s="10"/>
+      <c r="I81" s="10"/>
+      <c r="J81" s="10"/>
+    </row>
+    <row r="83" spans="1:10" ht="20.149999999999999" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A83" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="85" spans="1:10" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B85" s="19"/>
+      <c r="C85" s="19"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="19"/>
+      <c r="G85" s="19"/>
+    </row>
+    <row r="86" spans="1:10" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="20"/>
+      <c r="B86" s="20"/>
+      <c r="C86" s="20"/>
+      <c r="D86" s="20"/>
+      <c r="E86" s="20"/>
+      <c r="F86" s="20"/>
+      <c r="G86" s="20"/>
+    </row>
+    <row r="87" spans="1:10" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="20"/>
+      <c r="B87" s="20"/>
+      <c r="C87" s="20"/>
+      <c r="D87" s="20"/>
+      <c r="E87" s="20"/>
+      <c r="F87" s="20"/>
+      <c r="G87" s="20"/>
+    </row>
+    <row r="88" spans="1:10" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="20"/>
+      <c r="B88" s="20"/>
+      <c r="C88" s="20"/>
+      <c r="D88" s="20"/>
+      <c r="E88" s="20"/>
+      <c r="F88" s="20"/>
+      <c r="G88" s="20"/>
+    </row>
+    <row r="89" spans="1:10" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="20"/>
+      <c r="B89" s="20"/>
+      <c r="C89" s="20"/>
+      <c r="D89" s="20"/>
+      <c r="E89" s="20"/>
+      <c r="F89" s="20"/>
+      <c r="G89" s="20"/>
+    </row>
+    <row r="90" spans="1:10" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="20"/>
+      <c r="B90" s="20"/>
+      <c r="C90" s="20"/>
+      <c r="D90" s="20"/>
+      <c r="E90" s="20"/>
+      <c r="F90" s="20"/>
+      <c r="G90" s="20"/>
+    </row>
+    <row r="91" spans="1:10" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="20"/>
+      <c r="B91" s="20"/>
+      <c r="C91" s="20"/>
+      <c r="D91" s="20"/>
+      <c r="E91" s="20"/>
+      <c r="F91" s="20"/>
+      <c r="G91" s="20"/>
+    </row>
+    <row r="92" spans="1:10" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A92" s="20"/>
+      <c r="B92" s="20"/>
+      <c r="C92" s="20"/>
+      <c r="D92" s="20"/>
+      <c r="E92" s="20"/>
+      <c r="F92" s="20"/>
+      <c r="G92" s="20"/>
+    </row>
+    <row r="93" spans="1:10" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A93" s="20"/>
+      <c r="B93" s="20"/>
+      <c r="C93" s="20"/>
+      <c r="D93" s="20"/>
+      <c r="E93" s="20"/>
+      <c r="F93" s="20"/>
+      <c r="G93" s="20"/>
+    </row>
+    <row r="94" spans="1:10" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="20"/>
+      <c r="B94" s="20"/>
+      <c r="C94" s="20"/>
+      <c r="D94" s="20"/>
+      <c r="E94" s="20"/>
+      <c r="F94" s="20"/>
+      <c r="G94" s="20"/>
+    </row>
+    <row r="95" spans="1:10" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A95" s="20"/>
+      <c r="B95" s="20"/>
+      <c r="C95" s="20"/>
+      <c r="D95" s="20"/>
+      <c r="E95" s="20"/>
+      <c r="F95" s="20"/>
+      <c r="G95" s="20"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A96" s="20"/>
+      <c r="B96" s="20"/>
+      <c r="C96" s="20"/>
+      <c r="D96" s="20"/>
+      <c r="E96" s="20"/>
+      <c r="F96" s="20"/>
+      <c r="G96" s="20"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A97" s="20"/>
+      <c r="B97" s="20"/>
+      <c r="C97" s="20"/>
+      <c r="D97" s="20"/>
+      <c r="E97" s="20"/>
+      <c r="F97" s="20"/>
+      <c r="G97" s="20"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A98" s="20"/>
+      <c r="B98" s="20"/>
+      <c r="C98" s="20"/>
+      <c r="D98" s="20"/>
+      <c r="E98" s="20"/>
+      <c r="F98" s="20"/>
+      <c r="G98" s="20"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A99" s="20"/>
+      <c r="B99" s="20"/>
+      <c r="C99" s="20"/>
+      <c r="D99" s="20"/>
+      <c r="E99" s="20"/>
+      <c r="F99" s="20"/>
+      <c r="G99" s="20"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A100" s="20"/>
+      <c r="B100" s="20"/>
+      <c r="C100" s="20"/>
+      <c r="D100" s="20"/>
+      <c r="E100" s="20"/>
+      <c r="F100" s="20"/>
+      <c r="G100" s="20"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A101" s="20"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20"/>
+      <c r="D101" s="20"/>
+      <c r="E101" s="20"/>
+      <c r="F101" s="20"/>
+      <c r="G101" s="20"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A102" s="20"/>
+      <c r="B102" s="20"/>
+      <c r="C102" s="20"/>
+      <c r="D102" s="20"/>
+      <c r="E102" s="20"/>
+      <c r="F102" s="20"/>
+      <c r="G102" s="20"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A103" s="9" t="str" cm="1">
+        <f t="array" ref="A103:C108">_xll.DuckDbQuery(A85)</f>
+        <v>Country</v>
+      </c>
+      <c r="B103" s="9" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="C103" s="9" t="str">
+        <v>Nobel Laureates</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A104" t="str">
+        <v>USA</v>
+      </c>
+      <c r="B104" s="4">
+        <v>24745402581.060123</v>
+      </c>
+      <c r="C104">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A105" t="str">
+        <v>United Kingdom</v>
+      </c>
+      <c r="B105" s="4">
+        <v>7491539226.9900084</v>
+      </c>
+      <c r="C105">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A106" t="str">
+        <v>Germany</v>
+      </c>
+      <c r="B106" s="4">
+        <v>5857271880.1199961</v>
+      </c>
+      <c r="C106">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A107" t="str">
+        <v>France</v>
+      </c>
+      <c r="B107" s="4">
+        <v>4059423265.9799981</v>
+      </c>
+      <c r="C107">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A108" t="str">
+        <v>Sweden</v>
+      </c>
+      <c r="B108" s="4">
+        <v>2035288134.5999994</v>
+      </c>
+      <c r="C108">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="D1:L4"/>
+    <mergeCell ref="D10:L13"/>
+    <mergeCell ref="D19:L25"/>
+    <mergeCell ref="A85:G102"/>
     <mergeCell ref="D71:J75"/>
     <mergeCell ref="F77:J81"/>
     <mergeCell ref="D37:J41"/>
     <mergeCell ref="D46:J48"/>
     <mergeCell ref="D59:J64"/>
-    <mergeCell ref="D1:L4"/>
-    <mergeCell ref="D10:L13"/>
-    <mergeCell ref="D19:L25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" xr:uid="{F0FED8AF-9214-4F4A-B875-5FCE6FEEB4B5}"/>

</xml_diff>